<commit_message>
immune analysis updates II
</commit_message>
<xml_diff>
--- a/immune_data/observations.xlsx
+++ b/immune_data/observations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="removed" sheetId="1" state="visible" r:id="rId3"/>
@@ -650,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:Z1118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A261" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B286" activeCellId="0" sqref="B286"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12352,8 +12352,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
readme edit, added author
</commit_message>
<xml_diff>
--- a/immune_data/observations.xlsx
+++ b/immune_data/observations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="removed" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="119">
   <si>
     <t xml:space="preserve">datetime</t>
   </si>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">21</t>
   </si>
   <si>
-    <t xml:space="preserve">feed emptied; censored</t>
+    <t xml:space="preserve">incubator malfunction; censored</t>
   </si>
   <si>
     <t xml:space="preserve">20</t>
@@ -308,13 +308,7 @@
     <t xml:space="preserve">all dead</t>
   </si>
   <si>
-    <t xml:space="preserve">incubator turned off (malfunction)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incubator turned off &amp; very sticky</t>
-  </si>
-  <si>
-    <t xml:space="preserve">incubator turned off; escaped :(</t>
+    <t xml:space="preserve">sticky</t>
   </si>
   <si>
     <t xml:space="preserve">escape</t>
@@ -650,8 +644,8 @@
   </sheetPr>
   <dimension ref="A1:Z1118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B228" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J257" activeCellId="0" sqref="J257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7810,9 +7804,7 @@
       <c r="F343" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G343" s="7" t="s">
-        <v>95</v>
-      </c>
+      <c r="G343" s="7"/>
     </row>
     <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A344" s="8" t="n">
@@ -7834,7 +7826,7 @@
         <v>40</v>
       </c>
       <c r="G344" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7857,7 +7849,7 @@
         <v>40</v>
       </c>
       <c r="G345" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7880,7 +7872,7 @@
         <v>40</v>
       </c>
       <c r="G346" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7903,7 +7895,7 @@
         <v>40</v>
       </c>
       <c r="G347" s="7" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7926,7 +7918,7 @@
         <v>40</v>
       </c>
       <c r="G348" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7948,9 +7940,7 @@
       <c r="F349" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G349" s="7" t="s">
-        <v>95</v>
-      </c>
+      <c r="G349" s="7"/>
     </row>
     <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A350" s="8" t="n">
@@ -7971,9 +7961,7 @@
       <c r="F350" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G350" s="7" t="s">
-        <v>95</v>
-      </c>
+      <c r="G350" s="7"/>
     </row>
     <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A351" s="8" t="n">
@@ -8195,7 +8183,7 @@
         <v>34</v>
       </c>
       <c r="G361" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8318,7 +8306,7 @@
         <v>40</v>
       </c>
       <c r="G367" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8384,7 +8372,7 @@
         <v>40</v>
       </c>
       <c r="G370" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8476,7 +8464,7 @@
         <v>40</v>
       </c>
       <c r="G374" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8748,7 +8736,7 @@
         <v>40</v>
       </c>
       <c r="G387" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8831,7 +8819,7 @@
         <v>40</v>
       </c>
       <c r="G391" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8854,7 +8842,7 @@
         <v>40</v>
       </c>
       <c r="G392" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8877,7 +8865,7 @@
         <v>40</v>
       </c>
       <c r="G393" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8900,7 +8888,7 @@
         <v>40</v>
       </c>
       <c r="G394" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9226,7 +9214,7 @@
         <v>40</v>
       </c>
       <c r="G410" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="411" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9249,7 +9237,7 @@
         <v>40</v>
       </c>
       <c r="G411" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9272,7 +9260,7 @@
         <v>40</v>
       </c>
       <c r="G412" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9355,7 +9343,7 @@
         <v>40</v>
       </c>
       <c r="G416" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9378,7 +9366,7 @@
         <v>40</v>
       </c>
       <c r="G417" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9401,7 +9389,7 @@
         <v>40</v>
       </c>
       <c r="G418" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9424,7 +9412,7 @@
         <v>40</v>
       </c>
       <c r="G419" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9507,7 +9495,7 @@
         <v>40</v>
       </c>
       <c r="G423" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9530,7 +9518,7 @@
         <v>40</v>
       </c>
       <c r="G424" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9593,7 +9581,7 @@
         <v>34</v>
       </c>
       <c r="G427" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9876,7 +9864,7 @@
         <v>40</v>
       </c>
       <c r="G441" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9899,7 +9887,7 @@
         <v>40</v>
       </c>
       <c r="G442" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9922,7 +9910,7 @@
         <v>40</v>
       </c>
       <c r="G443" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10363,7 +10351,7 @@
         <v>34</v>
       </c>
       <c r="G464" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10469,7 +10457,7 @@
         <v>34</v>
       </c>
       <c r="G469" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10646,7 +10634,7 @@
         <v>40</v>
       </c>
       <c r="G478" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10709,7 +10697,7 @@
         <v>40</v>
       </c>
       <c r="G481" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11158,7 +11146,7 @@
         <v>34</v>
       </c>
       <c r="G503" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H503" s="1"/>
       <c r="I503" s="1"/>
@@ -11320,7 +11308,7 @@
         <v>34</v>
       </c>
       <c r="G509" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11546,7 +11534,7 @@
         <v>34</v>
       </c>
       <c r="G520" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11623,7 +11611,7 @@
         <v>34</v>
       </c>
       <c r="G524" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12352,7 +12340,7 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B44" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -12368,22 +12356,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -12398,7 +12386,7 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>18</v>
@@ -12420,7 +12408,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>20</v>
@@ -12442,7 +12430,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>25</v>
@@ -12464,7 +12452,7 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>18</v>
@@ -12486,7 +12474,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>20</v>
@@ -12508,7 +12496,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>18</v>
@@ -12530,7 +12518,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>25</v>
@@ -12552,7 +12540,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>20</v>
@@ -12574,7 +12562,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>25</v>
@@ -12596,7 +12584,7 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>40</v>
@@ -12618,7 +12606,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>43</v>
@@ -12640,7 +12628,7 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>42</v>
@@ -12662,7 +12650,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E14" s="3" t="n">
         <v>44</v>
@@ -12684,7 +12672,7 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E15" s="3" t="n">
         <v>40</v>
@@ -12706,7 +12694,7 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E16" s="3" t="n">
         <v>43</v>
@@ -12728,7 +12716,7 @@
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E17" s="3" t="n">
         <v>42</v>
@@ -12750,7 +12738,7 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>44</v>
@@ -12772,7 +12760,7 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>40</v>
@@ -12794,7 +12782,7 @@
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>44</v>
@@ -12816,7 +12804,7 @@
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>42</v>
@@ -12838,7 +12826,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E22" s="3" t="n">
         <v>43</v>
@@ -12860,7 +12848,7 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>40</v>
@@ -12882,7 +12870,7 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E24" s="3" t="n">
         <v>42</v>
@@ -12904,7 +12892,7 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>44</v>
@@ -12926,7 +12914,7 @@
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>43</v>
@@ -12948,7 +12936,7 @@
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>28</v>
@@ -12969,7 +12957,7 @@
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>28</v>
@@ -12990,7 +12978,7 @@
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>28</v>
@@ -13011,7 +12999,7 @@
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E30" s="3" t="n">
         <v>32</v>
@@ -13032,7 +13020,7 @@
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>28</v>
@@ -13053,7 +13041,7 @@
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>29</v>
@@ -13074,7 +13062,7 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E33" s="3" t="n">
         <v>28</v>
@@ -13095,7 +13083,7 @@
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E34" s="3" t="n">
         <v>32</v>
@@ -13116,7 +13104,7 @@
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E35" s="3" t="n">
         <v>28</v>
@@ -13137,7 +13125,7 @@
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E36" s="3" t="n">
         <v>29</v>
@@ -13158,7 +13146,7 @@
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E37" s="3" t="n">
         <v>29</v>
@@ -13179,7 +13167,7 @@
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>29</v>
@@ -13200,7 +13188,7 @@
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E39" s="3" t="n">
         <v>29</v>
@@ -13221,7 +13209,7 @@
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E40" s="3" t="n">
         <v>32</v>
@@ -13242,7 +13230,7 @@
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E41" s="3" t="n">
         <v>29</v>
@@ -13263,7 +13251,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E42" s="3" t="n">
         <v>32</v>
@@ -13284,7 +13272,7 @@
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E43" s="3" t="n">
         <v>32</v>
@@ -13305,7 +13293,7 @@
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E44" s="3" t="n">
         <v>32</v>
@@ -13328,7 +13316,7 @@
         <v>45170.5</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E45" s="3" t="n">
         <v>40</v>
@@ -13351,7 +13339,7 @@
         <v>45170.5</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E46" s="3" t="n">
         <v>40</v>
@@ -13374,7 +13362,7 @@
         <v>45170.5</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E47" s="3" t="n">
         <v>42</v>
@@ -13397,7 +13385,7 @@
         <v>45170.5</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E48" s="3" t="n">
         <v>40</v>
@@ -13420,7 +13408,7 @@
         <v>45170.5</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E49" s="3" t="n">
         <v>43</v>
@@ -13443,7 +13431,7 @@
         <v>45170.5</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E50" s="3" t="n">
         <v>40</v>
@@ -13466,7 +13454,7 @@
         <v>45170.5</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E51" s="3" t="n">
         <v>44</v>
@@ -13489,7 +13477,7 @@
         <v>45170.5</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E52" s="3" t="n">
         <v>42</v>
@@ -13512,7 +13500,7 @@
         <v>45170.5</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E53" s="3" t="n">
         <v>42</v>
@@ -13535,7 +13523,7 @@
         <v>45170.5</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E54" s="3" t="n">
         <v>44</v>
@@ -13558,7 +13546,7 @@
         <v>45170.5</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E55" s="3" t="n">
         <v>42</v>
@@ -13581,7 +13569,7 @@
         <v>45170.5</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E56" s="3" t="n">
         <v>43</v>
@@ -13593,7 +13581,7 @@
         <v>2</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13607,7 +13595,7 @@
         <v>45170.5</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E57" s="3" t="n">
         <v>43</v>
@@ -13619,7 +13607,7 @@
         <v>2</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13633,7 +13621,7 @@
         <v>45170.5</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E58" s="3" t="n">
         <v>43</v>
@@ -13656,7 +13644,7 @@
         <v>45170.5</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E59" s="3" t="n">
         <v>44</v>
@@ -13668,7 +13656,7 @@
         <v>2</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13682,7 +13670,7 @@
         <v>45170.5</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E60" s="3" t="n">
         <v>44</v>
@@ -13694,7 +13682,7 @@
         <v>2</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13708,7 +13696,7 @@
         <v>45175.5</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E61" s="3" t="n">
         <v>18</v>
@@ -13731,7 +13719,7 @@
         <v>45175.5</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E62" s="3" t="n">
         <v>18</v>
@@ -13754,7 +13742,7 @@
         <v>45175.5</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E63" s="3" t="n">
         <v>19</v>
@@ -13777,7 +13765,7 @@
         <v>45175.5</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E64" s="3" t="n">
         <v>18</v>
@@ -13800,7 +13788,7 @@
         <v>45175.5</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E65" s="3" t="n">
         <v>20</v>
@@ -13823,7 +13811,7 @@
         <v>45175.5</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E66" s="3" t="n">
         <v>18</v>
@@ -13846,7 +13834,7 @@
         <v>45175.5</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E67" s="3" t="n">
         <v>22</v>
@@ -13869,7 +13857,7 @@
         <v>45175.5</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E68" s="3" t="n">
         <v>19</v>
@@ -13892,7 +13880,7 @@
         <v>45175.5</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E69" s="3" t="n">
         <v>19</v>
@@ -13915,7 +13903,7 @@
         <v>45175.5</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E70" s="3" t="n">
         <v>20</v>
@@ -13938,7 +13926,7 @@
         <v>45175.5</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E71" s="3" t="n">
         <v>19</v>
@@ -13961,7 +13949,7 @@
         <v>45175.5</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E72" s="3" t="n">
         <v>22</v>
@@ -13984,7 +13972,7 @@
         <v>45175.5</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E73" s="3" t="n">
         <v>20</v>
@@ -14007,7 +13995,7 @@
         <v>45175.5</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E74" s="3" t="n">
         <v>20</v>
@@ -14030,7 +14018,7 @@
         <v>45175.5</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E75" s="3" t="n">
         <v>22</v>
@@ -14053,7 +14041,7 @@
         <v>45175.5</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E76" s="3" t="n">
         <v>22</v>
@@ -14074,7 +14062,7 @@
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E77" s="3" t="n">
         <v>40</v>
@@ -14095,7 +14083,7 @@
       </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E78" s="3" t="n">
         <v>40</v>
@@ -14107,7 +14095,7 @@
         <v>4</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14119,7 +14107,7 @@
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E79" s="3" t="n">
         <v>42</v>
@@ -14131,7 +14119,7 @@
         <v>4</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14143,7 +14131,7 @@
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E80" s="3" t="n">
         <v>40</v>
@@ -14164,7 +14152,7 @@
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E81" s="3" t="n">
         <v>43</v>
@@ -14185,7 +14173,7 @@
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E82" s="3" t="n">
         <v>40</v>
@@ -14206,7 +14194,7 @@
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E83" s="3" t="n">
         <v>44</v>
@@ -14227,7 +14215,7 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E84" s="3" t="n">
         <v>42</v>
@@ -14248,7 +14236,7 @@
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E85" s="3" t="n">
         <v>42</v>
@@ -14260,7 +14248,7 @@
         <v>4</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14272,7 +14260,7 @@
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E86" s="3" t="n">
         <v>43</v>
@@ -14293,7 +14281,7 @@
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E87" s="3" t="n">
         <v>42</v>
@@ -14314,7 +14302,7 @@
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E88" s="3" t="n">
         <v>44</v>
@@ -14335,7 +14323,7 @@
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E89" s="3" t="n">
         <v>43</v>
@@ -14356,7 +14344,7 @@
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E90" s="3" t="n">
         <v>43</v>
@@ -14377,7 +14365,7 @@
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E91" s="3" t="n">
         <v>44</v>
@@ -14398,7 +14386,7 @@
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E92" s="3" t="n">
         <v>44</v>
@@ -14419,7 +14407,7 @@
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E93" s="3" t="n">
         <v>19</v>
@@ -14440,7 +14428,7 @@
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E94" s="3" t="n">
         <v>19</v>
@@ -14461,7 +14449,7 @@
       </c>
       <c r="C95" s="3"/>
       <c r="D95" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E95" s="3" t="n">
         <v>20</v>
@@ -14482,7 +14470,7 @@
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E96" s="3" t="n">
         <v>19</v>
@@ -14503,7 +14491,7 @@
       </c>
       <c r="C97" s="3"/>
       <c r="D97" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E97" s="3" t="n">
         <v>22</v>
@@ -14524,7 +14512,7 @@
       </c>
       <c r="C98" s="3"/>
       <c r="D98" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E98" s="3" t="n">
         <v>20</v>
@@ -14545,7 +14533,7 @@
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E99" s="3" t="n">
         <v>20</v>
@@ -14566,7 +14554,7 @@
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E100" s="3" t="n">
         <v>22</v>
@@ -14587,7 +14575,7 @@
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E101" s="3" t="n">
         <v>22</v>
@@ -14608,7 +14596,7 @@
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E102" s="3" t="n">
         <v>17</v>
@@ -14629,7 +14617,7 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E103" s="3" t="n">
         <v>17</v>
@@ -14650,7 +14638,7 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E104" s="3" t="n">
         <v>19</v>
@@ -14671,7 +14659,7 @@
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E105" s="3" t="n">
         <v>17</v>
@@ -14692,7 +14680,7 @@
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E106" s="3" t="n">
         <v>20</v>
@@ -14713,7 +14701,7 @@
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E107" s="3" t="n">
         <v>17</v>
@@ -14734,7 +14722,7 @@
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E108" s="3" t="n">
         <v>22</v>

</xml_diff>